<commit_message>
almost done with music demo
</commit_message>
<xml_diff>
--- a/UIST2021/Eval/GazeResults.xlsx
+++ b/UIST2021/Eval/GazeResults.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karanahuja/Dropbox/GAZEL/UIST2021/Eval/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andykong/Dropbox/GAZEL/UIST2021/Eval/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BE4623-0162-B041-93C9-B6AA6D514881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19080" activeTab="1" xr2:uid="{E8D15233-9FE9-ED43-ABCC-130BE089DC4C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,9 +31,15 @@
     <definedName name="_xlchart.v1.8" hidden="1">Sheet2!$B$1</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">Sheet2!$B$2:$B$11</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -50,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Window Size</t>
   </si>
@@ -72,12 +77,45 @@
   <si>
     <t>Y Error</t>
   </si>
+  <si>
+    <t>a = np.array([[367,   2,   4,   0,   0,   3,   3,   0,   0],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       [  0, 364,  32,   1,   0,   0,   0,   2,   0],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       [  0,   3, 307,   0,   0,   0,   1,   8,   0],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       [  0,   1,   2, 363,  18,   0,   0,   0,  10],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       [  0,   0,   0,   1, 337,   0,   0,   0,   1],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       [  0,   0,   0,   0,   0, 328,   0,   0,   0],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       [  0,   0,   2,   0,   3,   2, 359,   1,   0],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       [  0,   0,   8,   0,   0,   0,   0, 336,   1],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       [  0,   0,   0,   2,   4,   0,   0,  26, 361]])</t>
+  </si>
+  <si>
+    <t>Confusion Matrix</t>
+  </si>
+  <si>
+    <t>gestLabels = ["Forward flick", "Right flick", "Right tilt", "Left flick", "Left tilt", "Pull close", "Push away", "Turn to right", "Turn to left"];</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -154,7 +192,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -331,34 +369,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400</c:v>
+                  <c:v>400.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600</c:v>
+                  <c:v>600.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700</c:v>
+                  <c:v>700.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800</c:v>
+                  <c:v>800.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -373,10 +411,10 @@
                   <c:v>2.58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4900000000000002</c:v>
+                  <c:v>2.49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2400000000000002</c:v>
+                  <c:v>2.24</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.08</c:v>
@@ -402,7 +440,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-74B6-8D45-B901-941FD1E96755}"/>
             </c:ext>
@@ -418,11 +456,11 @@
         </c:dLbls>
         <c:gapWidth val="80"/>
         <c:overlap val="-75"/>
-        <c:axId val="1147425920"/>
-        <c:axId val="1147443696"/>
+        <c:axId val="1309725312"/>
+        <c:axId val="1309729712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1147425920"/>
+        <c:axId val="1309725312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -525,7 +563,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1147443696"/>
+        <c:crossAx val="1309729712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -533,7 +571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1147443696"/>
+        <c:axId val="1309729712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -584,7 +622,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1147425920"/>
+        <c:crossAx val="1309725312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -629,7 +667,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -776,34 +814,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400</c:v>
+                  <c:v>400.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600</c:v>
+                  <c:v>600.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700</c:v>
+                  <c:v>700.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800</c:v>
+                  <c:v>800.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -815,10 +853,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>0.56</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.54</c:v>
@@ -847,7 +885,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-946A-EE4C-80B5-486AB67D88D2}"/>
             </c:ext>
@@ -980,34 +1018,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400</c:v>
+                  <c:v>400.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600</c:v>
+                  <c:v>600.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700</c:v>
+                  <c:v>700.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800</c:v>
+                  <c:v>800.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1019,10 +1057,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.4300000000000002</c:v>
+                  <c:v>2.43</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.09</c:v>
@@ -1051,7 +1089,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-946A-EE4C-80B5-486AB67D88D2}"/>
             </c:ext>
@@ -1184,34 +1222,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400</c:v>
+                  <c:v>400.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600</c:v>
+                  <c:v>600.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700</c:v>
+                  <c:v>700.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800</c:v>
+                  <c:v>800.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1226,10 +1264,10 @@
                   <c:v>2.58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4900000000000002</c:v>
+                  <c:v>2.49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2400000000000002</c:v>
+                  <c:v>2.24</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.08</c:v>
@@ -1255,7 +1293,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-946A-EE4C-80B5-486AB67D88D2}"/>
             </c:ext>
@@ -1270,11 +1308,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1144950928"/>
-        <c:axId val="1144338912"/>
+        <c:axId val="1309118960"/>
+        <c:axId val="1309123232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1144950928"/>
+        <c:axId val="1309118960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1325,6 +1363,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1391,7 +1430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1144338912"/>
+        <c:crossAx val="1309123232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1399,7 +1438,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1144338912"/>
+        <c:axId val="1309123232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1445,6 +1484,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1511,7 +1551,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1144950928"/>
+        <c:crossAx val="1309118960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1525,6 +1565,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -2709,7 +2750,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3690819-A387-1940-B12A-E0A1E5929B66}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D3690819-A387-1940-B12A-E0A1E5929B66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2750,7 +2791,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E384E78C-E83B-CA4C-BB69-94A1CE691721}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E384E78C-E83B-CA4C-BB69-94A1CE691721}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3067,26 +3108,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{163AB810-80F0-DB4B-90BD-788F52BED351}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -3094,7 +3135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>100</v>
       </c>
@@ -3105,7 +3146,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>200</v>
       </c>
@@ -3116,7 +3157,7 @@
         <v>1.59</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>300</v>
       </c>
@@ -3127,7 +3168,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>400</v>
       </c>
@@ -3138,7 +3179,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>500</v>
       </c>
@@ -3149,7 +3190,7 @@
         <v>1.41</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>600</v>
       </c>
@@ -3160,7 +3201,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>700</v>
       </c>
@@ -3171,7 +3212,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>800</v>
       </c>
@@ -3182,7 +3223,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>900</v>
       </c>
@@ -3193,7 +3234,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1000</v>
       </c>
@@ -3204,7 +3245,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -3212,52 +3253,52 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
     </row>
   </sheetData>
@@ -3267,21 +3308,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A92255F8-6050-D54F-A740-11AB96C0EB2F}">
-  <dimension ref="A1:H40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3295,7 +3336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>100</v>
       </c>
@@ -3318,7 +3359,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>200</v>
       </c>
@@ -3341,7 +3382,7 @@
         <v>1.59</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>300</v>
       </c>
@@ -3364,7 +3405,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>400</v>
       </c>
@@ -3387,7 +3428,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>500</v>
       </c>
@@ -3410,7 +3451,7 @@
         <v>1.41</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>600</v>
       </c>
@@ -3433,7 +3474,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>700</v>
       </c>
@@ -3456,7 +3497,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>800</v>
       </c>
@@ -3479,7 +3520,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>900</v>
       </c>
@@ -3502,7 +3543,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1000</v>
       </c>
@@ -3525,80 +3566,129 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="19">
+    <row r="16" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="3:3" ht="19">
+    <row r="17" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="3:3" ht="19">
+    <row r="18" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="3:3" ht="19">
+    <row r="19" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="3:3" ht="19">
+    <row r="20" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="3:3" ht="19">
+    <row r="21" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="3:3" ht="19">
+    <row r="22" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="3:3" ht="19">
+    <row r="23" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="3:3" ht="19">
+    <row r="24" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="3:3" ht="19">
+    <row r="25" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="3:3" ht="19">
+    <row r="26" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="3:3" ht="19">
+    <row r="27" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="3:3" ht="19">
+    <row r="28" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="3:3" ht="19">
+    <row r="29" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="3:3" ht="19">
+    <row r="30" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="3:3" ht="19">
+    <row r="31" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="3:3" ht="19">
+    <row r="32" spans="3:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="3:3" ht="19">
+    <row r="33" spans="2:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="3:3" ht="19">
+    <row r="34" spans="2:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="3:3" ht="19">
+    <row r="35" spans="2:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="3:3" ht="19">
+    <row r="36" spans="2:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="3:3" ht="19">
+    <row r="37" spans="2:3" ht="19" x14ac:dyDescent="0.25">
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="3:3" ht="19">
+    <row r="38" spans="2:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="3:3" ht="19">
+    <row r="39" spans="2:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="3:3" ht="19">
+    <row r="40" spans="2:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
       <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>